<commit_message>
Filtering works again. Also had to change minor naming error in years sheet in setup file
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v03_phe_06-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v03_phe_06-09-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9E7F84-025D-4C6E-8D1F-7BB38DF181E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0625E0CF-186F-4F4D-81DD-4273327B3A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -32,12 +32,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="262">
   <si>
     <t>DE</t>
   </si>
@@ -820,6 +831,9 @@
   </si>
   <si>
     <t>Region</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3403,17 +3417,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D817F8-1014-4E28-A827-54661E8BA006}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
user input adjustments in excel
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v03_phe_06-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v03_phe_06-09-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dozeumhep\Documents\git\GENeSYS-MOD_GroupRepo\GENeSYS-MOD_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0625E0CF-186F-4F4D-81DD-4273327B3A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E159838-42F4-4374-AE33-1D4B85A761EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -31,17 +31,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -885,7 +874,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -901,7 +890,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1199,11 +1188,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1222,7 +1211,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1238,7 +1227,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1254,7 +1243,7 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1278,7 +1267,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1286,7 +1275,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1542,7 +1531,7 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
@@ -1771,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>66</v>
       </c>
@@ -1779,7 +1768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>67</v>
       </c>
@@ -1787,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>68</v>
       </c>
@@ -1795,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>69</v>
       </c>
@@ -1803,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>70</v>
       </c>
@@ -2725,7 +2714,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -2812,7 +2801,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -3083,7 +3072,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -3138,7 +3127,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -3167,7 +3156,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -3334,7 +3323,7 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -3417,11 +3406,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D817F8-1014-4E28-A827-54661E8BA006}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>